<commit_message>
Ejobs + Linkdin + BestJobs - Working!
</commit_message>
<xml_diff>
--- a/JobScraping/config.xlsx
+++ b/JobScraping/config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Link</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>https://www.linkedin.com/jobs/</t>
+  </si>
+  <si>
+    <t>https://www.bestjobs.eu/ro/</t>
   </si>
 </sst>
 </file>
@@ -356,10 +359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -379,10 +382,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finalizarea functionalitatii de baza
</commit_message>
<xml_diff>
--- a/JobScraping/config.xlsx
+++ b/JobScraping/config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Link</t>
   </si>
@@ -31,6 +31,24 @@
   </si>
   <si>
     <t>https://www.bestjobs.eu/ro/</t>
+  </si>
+  <si>
+    <t>Paths</t>
+  </si>
+  <si>
+    <t>Ejobs.xlsx</t>
+  </si>
+  <si>
+    <t>Linkedin.xlsx</t>
+  </si>
+  <si>
+    <t>BestJobs.xlsx</t>
+  </si>
+  <si>
+    <t>AllJobs.xlsx</t>
+  </si>
+  <si>
+    <t>NewJobs.xlsx</t>
   </si>
 </sst>
 </file>
@@ -359,32 +377,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="72.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalizare detalii inaintea prezentarii
</commit_message>
<xml_diff>
--- a/JobScraping/config.xlsx
+++ b/JobScraping/config.xlsx
@@ -4,7 +4,7 @@
   <x:fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <x:workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="0" activeTab="0"/>
+    <x:workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <x:si>
     <x:t>Link</x:t>
   </x:si>
@@ -34,16 +34,22 @@
     <x:t>Last location</x:t>
   </x:si>
   <x:si>
+    <x:t>Email</x:t>
+  </x:si>
+  <x:si>
     <x:t>https://www.ejobs.ro/</x:t>
   </x:si>
   <x:si>
     <x:t>Ejobs.xlsx</x:t>
   </x:si>
   <x:si>
-    <x:t>babysitter</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bucuresti</x:t>
+    <x:t>C++</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cluj</x:t>
+  </x:si>
+  <x:si>
+    <x:t>catalinnm99@gmail.com</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.linkedin.com/jobs/</x:t>
@@ -112,8 +118,9 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="3">
+  <x:cellStyleXfs count="4">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -121,10 +128,11 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="5">
+  <x:cellXfs count="6">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -134,7 +142,8 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
-  <x:cellStyles count="1">
+  <x:cellStyles count="2">
+    <x:cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
   <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -415,79 +424,86 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D6"/>
+  <x:dimension ref="A1:E6"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="D2" sqref="D2 D2:D2"/>
+      <x:selection activeCell="E3" sqref="E3 E3:E3"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:cols>
-    <x:col min="1" max="1" width="72.886719" style="3" customWidth="1"/>
-    <x:col min="2" max="2" width="13.886719" style="3" customWidth="1"/>
-    <x:col min="3" max="3" width="22.332031" style="3" customWidth="1"/>
-    <x:col min="4" max="4" width="17.109375" style="3" customWidth="1"/>
+    <x:col min="1" max="1" width="72.886719" style="4" customWidth="1"/>
+    <x:col min="2" max="2" width="13.886719" style="4" customWidth="1"/>
+    <x:col min="3" max="3" width="22.332031" style="4" customWidth="1"/>
+    <x:col min="4" max="4" width="17.109375" style="4" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <x:c r="A1" s="3" t="s">
+    <x:row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <x:c r="A1" s="4" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="3" t="s">
+      <x:c r="B1" s="4" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="3" t="s">
+      <x:c r="C1" s="4" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="3" t="s">
+      <x:c r="D1" s="4" t="s">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="E1" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <x:c r="A2" s="4" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B2" s="3" t="s">
+    <x:row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <x:c r="A2" s="5" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="C2" s="3" t="s">
+      <x:c r="B2" s="4" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="D2" s="3" t="s">
+      <x:c r="C2" s="4" t="s">
         <x:v>7</x:v>
       </x:c>
+      <x:c r="D2" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E2" s="5" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
-    <x:row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <x:c r="A3" s="4" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B3" s="3" t="s">
-        <x:v>9</x:v>
+    <x:row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <x:c r="A3" s="5" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B3" s="4" t="s">
+        <x:v>11</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <x:c r="A4" s="4" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B4" s="3" t="s">
-        <x:v>11</x:v>
+    <x:row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <x:c r="A4" s="5" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B4" s="4" t="s">
+        <x:v>13</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <x:c r="B5" s="3" t="s">
-        <x:v>12</x:v>
+    <x:row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <x:c r="B5" s="4" t="s">
+        <x:v>14</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <x:c r="B6" s="3" t="s">
-        <x:v>13</x:v>
+    <x:row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <x:c r="B6" s="4" t="s">
+        <x:v>15</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="A2" r:id="rId8"/>
-    <x:hyperlink ref="A3" r:id="rId9"/>
-    <x:hyperlink ref="A4" r:id="rId10"/>
+    <x:hyperlink ref="A2" r:id="rId9"/>
+    <x:hyperlink ref="A3" r:id="rId10"/>
+    <x:hyperlink ref="A4" r:id="rId11"/>
+    <x:hyperlink ref="E2" r:id="rId12"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>